<commit_message>
Fixed separate blue-word coordinate output problem
Output sheets now group blue words if they are in the same brackets. Also ran the script to generate outputs.
</commit_message>
<xml_diff>
--- a/articles/article6/article_sheet.xlsx
+++ b/articles/article6/article_sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\text_and_image_processing\article_generation\jamario_new\articles\article6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\text_and_image_processing\article_generation\gitversion\articles\article6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8FC46A-B9F9-4DE4-BD03-83F35178FA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FA7F28-325E-4541-A542-B650F0CD160B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="2895" windowWidth="24090" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -126,13 +126,13 @@
     <t>article6.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">This was the second of two revolutions in the Russian Revolution. The first part was the [February Revolution . The second was the [October Revolution]. </t>
-  </si>
-  <si>
     <t>Some Russians did not like the previous [czarist government].</t>
   </si>
   <si>
     <t xml:space="preserve">They created the white army and fought Lenin and his red army. This was the [Russian Civil War]. Lenin won, and so the communist [Soviet Union] was born. This was the start of communist rule in Russia. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This was the second of two revolutions in the Russian Revolution. The first part was the [February Revolution]. The second was the [October Revolution]. </t>
   </si>
 </sst>
 </file>
@@ -458,19 +458,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="86.88671875" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="86.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,7 +487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -504,7 +504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -521,7 +521,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -538,7 +538,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -555,7 +555,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -572,7 +572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -589,7 +589,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -606,7 +606,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -620,27 +620,27 @@
         <v>400</v>
       </c>
       <c r="E9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>400</v>
+      </c>
+      <c r="E10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10">
-        <v>400</v>
-      </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -657,7 +657,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -674,7 +674,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -691,7 +691,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -708,7 +708,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -725,7 +725,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -742,7 +742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -759,7 +759,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -776,7 +776,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -793,7 +793,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -807,10 +807,10 @@
         <v>400</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Create CSV from excel files
</commit_message>
<xml_diff>
--- a/articles/article6/article_sheet.xlsx
+++ b/articles/article6/article_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\text_and_image_processing\article_generation\gitversion\articles\article6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamariorankins/repos/article_study/articles/article6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FA7F28-325E-4541-A542-B650F0CD160B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B83CC19-2376-C14C-9743-61657269A9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="2895" windowWidth="24090" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12840" yWindow="3700" windowWidth="24100" windowHeight="11660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -459,18 +459,18 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="86.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="86.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,7 +487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -504,7 +504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -521,7 +521,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -538,7 +538,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -555,7 +555,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -572,7 +572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -589,7 +589,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -606,7 +606,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -623,7 +623,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -640,7 +640,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -657,7 +657,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -674,7 +674,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -691,7 +691,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -708,7 +708,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -725,7 +725,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -742,7 +742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -759,7 +759,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -776,7 +776,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -793,7 +793,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -810,7 +810,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>

</xml_diff>